<commit_message>
maven repository for apache poi 4.1.2 adapted is moved to gh-pages-dev.
</commit_message>
<xml_diff>
--- a/meta/program/BlancoMeta2XmlConstants.xlsx
+++ b/meta/program/BlancoMeta2XmlConstants.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10913"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/blanco/blancoMeta2Xml/meta/program/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EB81E93C-EB54-0343-A777-7944A7CAC3CE}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{826CA89B-D41A-CE48-BF7D-C0501D6C19AC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" tabRatio="640"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" tabRatio="640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="constants" sheetId="1" r:id="rId1"/>
@@ -33,15 +33,7 @@
     <definedName name="項目型">#REF!</definedName>
     <definedName name="必須">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="0" concurrentCalc="0"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -162,14 +154,14 @@
     <t>○</t>
   </si>
   <si>
-    <t>"2.0.2"</t>
+    <t>"2.1.1"</t>
     <phoneticPr fontId="4"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5">
     <font>
       <sz val="11"/>
@@ -1048,14 +1040,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:H33"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
@@ -1421,19 +1413,19 @@
   </mergeCells>
   <phoneticPr fontId="4"/>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="D47">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="D47" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>型</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="C12">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="C12" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>adjustConstValue</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="C11">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="C11" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>isAbstract</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="C10">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="C10" xr:uid="{00000000-0002-0000-0000-000003000000}">
       <formula1>accessScope</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -1447,7 +1439,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>